<commit_message>
Added correct reference traces
</commit_message>
<xml_diff>
--- a/reference_traces/Sfp1_PKA2D.xlsx
+++ b/reference_traces/Sfp1_PKA2D.xlsx
@@ -346,502 +346,502 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>2.6564497314321098</v>
+        <v>2.5303282475197002</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2.67787317024758</v>
+        <v>2.54318725804539</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2.6978962532856001</v>
+        <v>2.55633262086624</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2.7164147087511799</v>
+        <v>2.5709707003347599</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2.7352269483907499</v>
+        <v>2.5851627489545401</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2.7583027354581899</v>
+        <v>2.59342596145909</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2.7844670834999001</v>
+        <v>2.60162425409395</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2.8081945599776401</v>
+        <v>2.6188078153578398</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2.8277919421919799</v>
+        <v>2.64240060943599</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2.84230017609196</v>
+        <v>2.6688999520605501</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2.8513847145800599</v>
+        <v>2.6937108627031301</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2.8624321069648402</v>
+        <v>2.7058237660023599</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2.87533402683699</v>
+        <v>2.7121811026100402</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2.8877390993107102</v>
+        <v>2.7157002466516298</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2.8973022699706901</v>
+        <v>2.71854095924345</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2.9014395658750902</v>
+        <v>2.7219876639975902</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>2.9027019873985398</v>
+        <v>2.7239187288901001</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>2.9011375099225098</v>
+        <v>2.72359693305981</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>2.8998484245037801</v>
+        <v>2.7221034039346899</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>2.9000426187667299</v>
+        <v>2.7183511365078799</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>2.8995406767729901</v>
+        <v>2.7069797438571999</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>2.8945033656382</v>
+        <v>2.6947341612836602</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>2.8907827512867201</v>
+        <v>2.6883715962836199</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>2.8890768785356702</v>
+        <v>2.6848469037189302</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>2.88928274054435</v>
+        <v>2.6821331312997798</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>2.8904866225041301</v>
+        <v>2.6815362260294902</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>2.898945634755</v>
+        <v>2.68912185048121</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>2.90747615226375</v>
+        <v>2.6924721488391401</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>2.91332250365183</v>
+        <v>2.6920286680807801</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>2.91530021959823</v>
+        <v>2.68953240781914</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>2.9146193295202001</v>
+        <v>2.6871961071242501</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>2.9154395328272402</v>
+        <v>2.6848902085094499</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>2.9196566316836998</v>
+        <v>2.68337590327658</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>2.9272698307642901</v>
+        <v>2.68224870104561</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>2.93807285890197</v>
+        <v>2.6811214988146501</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>2.9524011300454198</v>
+        <v>2.6799942965836898</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>2.9632320530548899</v>
+        <v>2.67731031282108</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>2.9713532936001101</v>
+        <v>2.6770548278194202</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>2.9782694420008502</v>
+        <v>2.6793408213313299</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>2.9851745410547901</v>
+        <v>2.68339216378439</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>2.9918103964981699</v>
+        <v>2.68744350623744</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>2.9951513873178599</v>
+        <v>2.6915580984716301</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>2.9981211257855902</v>
+        <v>2.6954596007596399</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>3.0011041640521099</v>
+        <v>2.6979860951591701</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>3.0041606821926701</v>
+        <v>2.6987828441670101</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>3.0075441359086001</v>
+        <v>2.7008907197673402</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>3.0119073082000698</v>
+        <v>2.7036680410886</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>3.0147294923724299</v>
+        <v>2.7068457489673499</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>3.0158943024970699</v>
+        <v>2.71104098005046</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>3.0157298286982699</v>
+        <v>2.71686448538347</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>3.0141757033208698</v>
+        <v>2.72451014772663</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>3.01331747826171</v>
+        <v>2.7324519950528399</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>3.0124364070069198</v>
+        <v>2.7407027219714499</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>3.01242999392481</v>
+        <v>2.74893798753603</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>3.0142078996028601</v>
+        <v>2.75548833304325</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>3.0171190973651898</v>
+        <v>2.7513246132226299</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>3.0199456952274901</v>
+        <v>2.7456559443353599</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>3.0241293404007901</v>
+        <v>2.73892923640391</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>3.0316747512274</v>
+        <v>2.7324451417298201</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>3.04388786729622</v>
+        <v>2.7281110445201202</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>3.05749378881552</v>
+        <v>2.7304319448593701</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>3.0715797052554099</v>
+        <v>2.7393281660465498</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>3.0841355600764202</v>
+        <v>2.75087738855221</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>3.0946540383844798</v>
+        <v>2.76651371037135</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>3.1031778921101401</v>
+        <v>2.7880652334660798</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>3.1097491156777299</v>
+        <v>2.80939363193772</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>3.1167113011813399</v>
+        <v>2.8403633086779201</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>3.1235087261859902</v>
+        <v>2.8729774131315202</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>3.13087796909987</v>
+        <v>2.9039480715811501</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>3.1397392909934099</v>
+        <v>2.9319539064101798</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>3.1482708300696398</v>
+        <v>2.9601171756142901</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>3.1565086983205499</v>
+        <v>2.9841894389635</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>3.1639792243984002</v>
+        <v>3.0054419028049999</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>3.1709363419846799</v>
+        <v>3.0259618093058802</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>3.1781922921922501</v>
+        <v>3.04795993814056</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>3.1892772997432699</v>
+        <v>3.06842853759477</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>3.1994390080899802</v>
+        <v>3.0870683660279599</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>3.2082415966071198</v>
+        <v>3.0962848190277898</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>3.21585720587187</v>
+        <v>3.0975469466399201</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>3.22289264301022</v>
+        <v>3.0969099137031</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>3.2309950010752799</v>
+        <v>3.0950130483766598</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>3.2392535622321499</v>
+        <v>3.0938670858438901</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>3.2439213161374201</v>
+        <v>3.0917112326548302</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>3.2447262255129399</v>
+        <v>3.0859578547313098</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>3.2433573423366702</v>
+        <v>3.0735595811160898</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>3.2377057526457702</v>
+        <v>3.0527246140500401</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>3.2264874859355399</v>
+        <v>3.0266941751002099</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>3.2055536383599099</v>
+        <v>2.9994306786688099</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>3.1734758021381202</v>
+        <v>2.9693798857651701</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>3.1311056975343701</v>
+        <v>2.9314636673908399</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>3.0844671951392901</v>
+        <v>2.8855901033769702</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>3.0347372089762001</v>
+        <v>2.8388720474887901</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>2.9829994807623401</v>
+        <v>2.7919047972770499</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>2.93202325640471</v>
+        <v>2.7457355729117801</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>2.8859704827453001</v>
+        <v>2.7019201856068999</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>2.8411634272208199</v>
+        <v>2.6697865209429401</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>2.7964566174322099</v>
+        <v>2.63696568675197</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>2.7514725998205098</v>
+        <v>2.6039272488774601</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>2.7061873537103698</v>
+        <v>2.5708888110029502</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>2.6609021076002199</v>
+        <v>2.5378503731284399</v>
       </c>
     </row>
   </sheetData>

</xml_diff>